<commit_message>
graphviz isn not working
</commit_message>
<xml_diff>
--- a/very_simple_examples/SampleMLData.xlsx
+++ b/very_simple_examples/SampleMLData.xlsx
@@ -1,22 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28104"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewclark/repos/simple-machine-learning-examples/very_simple_examples/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="18195" windowHeight="12330"/>
+    <workbookView xWindow="17240" yWindow="1160" windowWidth="18200" windowHeight="12340" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="7">
   <si>
     <t>Height</t>
   </si>
@@ -131,12 +144,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -166,12 +179,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -377,16 +390,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G13:G14"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -400,7 +413,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>181</v>
       </c>
@@ -414,7 +427,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>177</v>
       </c>
@@ -428,7 +441,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>160</v>
       </c>
@@ -445,7 +458,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>154</v>
       </c>
@@ -459,7 +472,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>166</v>
       </c>
@@ -473,7 +486,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>190</v>
       </c>
@@ -487,7 +500,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>175</v>
       </c>
@@ -501,7 +514,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>177</v>
       </c>
@@ -515,7 +528,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>159</v>
       </c>
@@ -529,7 +542,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>171</v>
       </c>
@@ -543,7 +556,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>181</v>
       </c>
@@ -565,12 +578,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>190</v>
+      </c>
+      <c r="B2">
+        <v>70</v>
+      </c>
+      <c r="C2">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -581,7 +619,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>